<commit_message>
12-invest ham birinchi marta uchun yakunlandi
</commit_message>
<xml_diff>
--- a/tools_llm/invest12/12 invest Hisobot (AI chat uchun).xlsx
+++ b/tools_llm/invest12/12 invest Hisobot (AI chat uchun).xlsx
@@ -432,7 +432,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +448,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -456,7 +462,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -547,6 +553,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -609,13 +622,6 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom/>
@@ -924,436 +930,436 @@
     <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="30" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="35" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="35" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="20" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="21" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="25" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="23" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="26" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="27" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="28" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="29" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="30" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="31" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="32" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="33" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="34" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="35" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="35" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="37" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -4186,7 +4192,7 @@
       <c r="U99" s="94"/>
       <c r="V99" s="95"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="275.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="172.125">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="96"/>
@@ -4210,7 +4216,7 @@
       <c r="U100" s="103"/>
       <c r="V100" s="104"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="132">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="70.875">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="60" t="s">
@@ -4242,7 +4248,7 @@
       <c r="U101" s="94"/>
       <c r="V101" s="95"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="132">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="70.875">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="96"/>
@@ -4266,7 +4272,7 @@
       <c r="U102" s="103"/>
       <c r="V102" s="104"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="92.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="50.625">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="60" t="s">
@@ -4298,7 +4304,7 @@
       <c r="U103" s="94"/>
       <c r="V103" s="95"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="48">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="50.625">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="96"/>

</xml_diff>